<commit_message>
Improve integration test. Hot fixes.
</commit_message>
<xml_diff>
--- a/src/test/resources/ParentTest.xlsx
+++ b/src/test/resources/ParentTest.xlsx
@@ -19,17 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>FK_LINK_HEADER_2</t>
   </si>
   <si>
-    <t>HEADER1</t>
-  </si>
-  <si>
-    <t>HEADER3</t>
-  </si>
-  <si>
     <t>Data1</t>
   </si>
   <si>
@@ -42,9 +36,6 @@
     <t>Data3</t>
   </si>
   <si>
-    <t>Nam3</t>
-  </si>
-  <si>
     <t>User3</t>
   </si>
   <si>
@@ -94,6 +85,24 @@
   </si>
   <si>
     <t>About3</t>
+  </si>
+  <si>
+    <t>New1</t>
+  </si>
+  <si>
+    <t>New2</t>
+  </si>
+  <si>
+    <t>New3</t>
+  </si>
+  <si>
+    <t>Header3</t>
+  </si>
+  <si>
+    <t>Header1</t>
+  </si>
+  <si>
+    <t>Name3</t>
   </si>
 </sst>
 </file>
@@ -460,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -475,72 +484,83 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" t="str">
         <f>[1]!Table3[[#This Row],[Header8]]</f>
         <v>Data8</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" t="str">
         <f>[1]Sheet1!$B$4</f>
         <v>User8</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" t="str">
         <f>Table1[[#This Row],[Header5]]</f>
         <v>User5</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B5" t="str">
         <f>Sheet2!B2</f>
         <v>Data5</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B6" t="str">
         <f>A2</f>
         <v>Data1</v>
       </c>
       <c r="C6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
         <v>24</v>
       </c>
     </row>
@@ -566,46 +586,46 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>